<commit_message>
add: report view for validator
</commit_message>
<xml_diff>
--- a/database/tb_report.xlsx
+++ b/database/tb_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,17 +466,27 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>status</t>
+          <t>status_laporan</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>status_jurnal</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>feedback</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>validator_id</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>tanggal_laporan</t>
         </is>
       </c>
     </row>
@@ -484,160 +494,40 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
       <c r="C2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://ojs.co.id</t>
+          <t>jurnal.com</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>cahaya publikasi</t>
+          <t>jurnal</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>jurnal mencurigakan</t>
+          <t>tes</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>pending</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>eduhealth.com</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>eduhealth</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>karena jurnal mencurigakan</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>eduhenter.com</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>adjuhsdfdjs</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>fdhgjdfhg</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>sjdfbhjs</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>sdjhfjsd</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>jshdfjs</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>https://jurnal.ojs.co.id</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Jurnal Cahaya</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>2024-12-23 00:15:09</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
progress: validation feature --savedata
</commit_message>
<xml_diff>
--- a/database/tb_report.xlsx
+++ b/database/tb_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,7 +517,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>pending</t>
+          <t>review</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
@@ -529,6 +529,318 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>jurnal.com</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>jurnal</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>te</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>review</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>2024-12-23 23:00:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>jurnal.com</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>jurnal ku</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>tes</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>review</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>2024-12-23 23:00:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>eduhealth</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>jurnal</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>tes</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>review</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>2024-12-23 23:00:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>dhfgsd</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>dsfhsdf]dsfjs</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>sdfbjs</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>review</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>2024-12-23 23:32:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>dsjfhsjd</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>dfgkdfjg</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>fdkgjdf</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>review</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>2024-12-23 23:39:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>sdjhsdfdgid</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>fdjgdf</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>fdjgdjfg</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>review</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>2024-12-23 23:43:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>jjjj</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>jjjj</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>jjj</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>review</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>2024-12-23 23:49:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>dsjfhs]f</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>jjjj</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>jjj</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>2024-12-23 23:50:08</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>